<commit_message>
l1 dist knee asc
</commit_message>
<xml_diff>
--- a/CancerSVM_dbscan.xlsx
+++ b/CancerSVM_dbscan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shukl\Documents\GitHub\CancerAceFiltering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAFF432-3E3F-48FB-9CF3-52D4287DD879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B9415B-AD52-40E1-91F6-E9D7974D85D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="14" activeTab="18" xr2:uid="{17001702-3C6F-4149-BC22-539ABEDFA4DC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="14" activeTab="20" xr2:uid="{17001702-3C6F-4149-BC22-539ABEDFA4DC}"/>
   </bookViews>
   <sheets>
     <sheet name="CancerDT75" sheetId="3" state="hidden" r:id="rId1"/>
@@ -33,9 +33,10 @@
     <sheet name="Sheet3" sheetId="23" r:id="rId18"/>
     <sheet name="dbscanclust_l1pca" sheetId="24" r:id="rId19"/>
     <sheet name="Sheet1" sheetId="20" r:id="rId20"/>
-    <sheet name="ace recur eps svm 20 % " sheetId="17" state="hidden" r:id="rId21"/>
-    <sheet name="ace recur eps svm 75 percentile" sheetId="18" state="hidden" r:id="rId22"/>
-    <sheet name="ace recur eps 25%" sheetId="19" state="hidden" r:id="rId23"/>
+    <sheet name="knee_l1pca" sheetId="25" r:id="rId21"/>
+    <sheet name="ace recur eps svm 20 % " sheetId="17" state="hidden" r:id="rId22"/>
+    <sheet name="ace recur eps svm 75 percentile" sheetId="18" state="hidden" r:id="rId23"/>
+    <sheet name="ace recur eps 25%" sheetId="19" state="hidden" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="89">
   <si>
     <t>---------split 1 --------------------</t>
   </si>
@@ -513,7 +514,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,8 +619,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF212121"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -725,6 +731,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1129,7 +1141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1343,6 +1355,60 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1385,12 +1451,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1409,14 +1469,11 @@
     <xf numFmtId="0" fontId="4" fillId="17" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1433,68 +1490,47 @@
     <xf numFmtId="0" fontId="4" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10596,16 +10632,16 @@
         <v>0</v>
       </c>
       <c r="L1" s="39"/>
-      <c r="M1" s="109" t="s">
+      <c r="M1" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="109"/>
-      <c r="O1" s="109"/>
-      <c r="P1" s="109"/>
-      <c r="Q1" s="109"/>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
-      <c r="T1" s="109"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
+      <c r="P1" s="133"/>
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="133"/>
+      <c r="T1" s="133"/>
       <c r="U1" s="28" t="s">
         <v>12</v>
       </c>
@@ -11556,17 +11592,17 @@
         <v>2</v>
       </c>
       <c r="L11" s="24"/>
-      <c r="M11" s="102" t="s">
+      <c r="M11" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="103"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="103"/>
-      <c r="Q11" s="103"/>
-      <c r="R11" s="103"/>
-      <c r="S11" s="103"/>
-      <c r="T11" s="103"/>
-      <c r="U11" s="104"/>
+      <c r="N11" s="127"/>
+      <c r="O11" s="127"/>
+      <c r="P11" s="127"/>
+      <c r="Q11" s="127"/>
+      <c r="R11" s="127"/>
+      <c r="S11" s="127"/>
+      <c r="T11" s="127"/>
+      <c r="U11" s="128"/>
       <c r="W11" s="31"/>
       <c r="X11" s="30"/>
       <c r="Y11" s="30"/>
@@ -11675,16 +11711,16 @@
       <c r="K13" s="4">
         <v>6.8292679999999999</v>
       </c>
-      <c r="W13" s="110" t="s">
+      <c r="W13" s="134" t="s">
         <v>21</v>
       </c>
-      <c r="X13" s="111"/>
-      <c r="Y13" s="111"/>
-      <c r="Z13" s="111"/>
-      <c r="AA13" s="111"/>
-      <c r="AB13" s="111"/>
-      <c r="AC13" s="111"/>
-      <c r="AD13" s="112"/>
+      <c r="X13" s="135"/>
+      <c r="Y13" s="135"/>
+      <c r="Z13" s="135"/>
+      <c r="AA13" s="135"/>
+      <c r="AB13" s="135"/>
+      <c r="AC13" s="135"/>
+      <c r="AD13" s="136"/>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="3">
@@ -15381,16 +15417,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="108" t="s">
+      <c r="M1" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
+      <c r="N1" s="132"/>
+      <c r="O1" s="132"/>
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
+      <c r="R1" s="132"/>
+      <c r="S1" s="132"/>
+      <c r="T1" s="132"/>
       <c r="U1" s="10" t="s">
         <v>12</v>
       </c>
@@ -19287,16 +19323,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="108" t="s">
+      <c r="M1" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
+      <c r="N1" s="132"/>
+      <c r="O1" s="132"/>
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
+      <c r="R1" s="132"/>
+      <c r="S1" s="132"/>
+      <c r="T1" s="132"/>
       <c r="U1" s="10" t="s">
         <v>12</v>
       </c>
@@ -24091,26 +24127,26 @@
     <row r="2" spans="2:12" ht="15" thickBot="1">
       <c r="B2" s="73"/>
       <c r="C2" s="73"/>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="143" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="114"/>
+      <c r="E2" s="144"/>
       <c r="F2" s="76"/>
-      <c r="J2" s="113" t="s">
+      <c r="J2" s="143" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="114"/>
+      <c r="K2" s="144"/>
     </row>
     <row r="3" spans="2:12" ht="14.55" customHeight="1">
-      <c r="D3" s="117" t="s">
+      <c r="D3" s="139" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="118"/>
+      <c r="E3" s="140"/>
       <c r="F3" s="86"/>
-      <c r="J3" s="117" t="s">
+      <c r="J3" s="139" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="118"/>
+      <c r="K3" s="140"/>
     </row>
     <row r="4" spans="2:12" ht="15" thickBot="1">
       <c r="D4" s="77" t="s">
@@ -24128,7 +24164,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="14.55" customHeight="1">
-      <c r="B5" s="119" t="b">
+      <c r="B5" s="141" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="81" t="s">
@@ -24140,10 +24176,10 @@
       <c r="E5" s="80">
         <v>4.8</v>
       </c>
-      <c r="F5" s="115" t="s">
+      <c r="F5" s="137" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="119" t="b">
+      <c r="H5" s="141" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="81" t="s">
@@ -24155,12 +24191,12 @@
       <c r="K5" s="80">
         <v>4.2</v>
       </c>
-      <c r="L5" s="115" t="s">
+      <c r="L5" s="137" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15" thickBot="1">
-      <c r="B6" s="120"/>
+      <c r="B6" s="142"/>
       <c r="C6" s="82" t="s">
         <v>52</v>
       </c>
@@ -24170,8 +24206,8 @@
       <c r="E6" s="80">
         <v>72.8</v>
       </c>
-      <c r="F6" s="116"/>
-      <c r="H6" s="120"/>
+      <c r="F6" s="138"/>
+      <c r="H6" s="142"/>
       <c r="I6" s="82" t="s">
         <v>52</v>
       </c>
@@ -24181,7 +24217,7 @@
       <c r="K6" s="80">
         <v>70.400000000000006</v>
       </c>
-      <c r="L6" s="116"/>
+      <c r="L6" s="138"/>
     </row>
     <row r="7" spans="2:12" ht="28.8">
       <c r="D7" s="94" t="s">
@@ -24401,14 +24437,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="H5:H6"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -24441,26 +24477,26 @@
     <row r="2" spans="2:12" ht="15" thickBot="1">
       <c r="B2" s="73"/>
       <c r="C2" s="73"/>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="143" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="114"/>
+      <c r="E2" s="144"/>
       <c r="F2" s="76"/>
-      <c r="J2" s="113" t="s">
+      <c r="J2" s="143" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="114"/>
+      <c r="K2" s="144"/>
     </row>
     <row r="3" spans="2:12" ht="14.55" customHeight="1">
-      <c r="D3" s="117" t="s">
+      <c r="D3" s="139" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="118"/>
+      <c r="E3" s="140"/>
       <c r="F3" s="86"/>
-      <c r="J3" s="117" t="s">
+      <c r="J3" s="139" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="118"/>
+      <c r="K3" s="140"/>
     </row>
     <row r="4" spans="2:12" ht="15" thickBot="1">
       <c r="D4" s="77" t="s">
@@ -24478,7 +24514,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="14.55" customHeight="1">
-      <c r="B5" s="119" t="b">
+      <c r="B5" s="141" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="81" t="s">
@@ -24492,10 +24528,10 @@
         <f>D13</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="F5" s="115" t="s">
+      <c r="F5" s="137" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="119" t="b">
+      <c r="H5" s="141" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="81" t="s">
@@ -24507,12 +24543,12 @@
       <c r="K5" s="80">
         <v>4.2</v>
       </c>
-      <c r="L5" s="115" t="s">
+      <c r="L5" s="137" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15" thickBot="1">
-      <c r="B6" s="120"/>
+      <c r="B6" s="142"/>
       <c r="C6" s="82" t="s">
         <v>52</v>
       </c>
@@ -24524,8 +24560,8 @@
         <f>D14</f>
         <v>72.3</v>
       </c>
-      <c r="F6" s="116"/>
-      <c r="H6" s="120"/>
+      <c r="F6" s="138"/>
+      <c r="H6" s="142"/>
       <c r="I6" s="82" t="s">
         <v>52</v>
       </c>
@@ -24535,7 +24571,7 @@
       <c r="K6" s="80">
         <v>70.400000000000006</v>
       </c>
-      <c r="L6" s="116"/>
+      <c r="L6" s="138"/>
     </row>
     <row r="7" spans="2:12" ht="28.8">
       <c r="D7" s="94" t="s">
@@ -24772,8 +24808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8CD87D-F648-4BF3-845B-D067AC887F9E}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -24782,89 +24818,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1">
-      <c r="B1" s="124" t="s">
+      <c r="B1" s="145" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="125"/>
-      <c r="D1" s="126"/>
-      <c r="G1" s="124" t="s">
+      <c r="C1" s="146"/>
+      <c r="D1" s="147"/>
+      <c r="G1" s="145" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="125"/>
-      <c r="I1" s="126"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="147"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1"/>
     <row r="3" spans="1:14" ht="15" thickBot="1">
       <c r="A3" s="74"/>
       <c r="B3" s="74"/>
-      <c r="C3" s="127" t="s">
+      <c r="C3" s="148" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="128"/>
-      <c r="E3" s="129"/>
-      <c r="H3" s="130" t="s">
+      <c r="D3" s="149"/>
+      <c r="E3" s="99"/>
+      <c r="H3" s="150" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="131"/>
+      <c r="I3" s="151"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
       <c r="A4" s="74"/>
       <c r="B4" s="74"/>
-      <c r="C4" s="132" t="s">
+      <c r="C4" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="133" t="s">
+      <c r="D4" s="101" t="s">
         <v>52</v>
       </c>
       <c r="G4" s="74"/>
-      <c r="H4" s="132" t="s">
+      <c r="H4" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="133" t="s">
+      <c r="I4" s="101" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="134" t="b">
+      <c r="A5" s="152" t="b">
         <v>1</v>
       </c>
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="136">
+      <c r="C5" s="103">
         <v>127.3</v>
       </c>
-      <c r="D5" s="137">
+      <c r="D5" s="104">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G5" s="135" t="s">
+      <c r="G5" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="136">
+      <c r="H5" s="103">
         <v>127.2</v>
       </c>
-      <c r="I5" s="137">
+      <c r="I5" s="104">
         <v>4.2</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1">
-      <c r="A6" s="138"/>
-      <c r="B6" s="139" t="s">
+      <c r="A6" s="153"/>
+      <c r="B6" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="140">
+      <c r="C6" s="106">
         <v>2.4</v>
       </c>
-      <c r="D6" s="141">
+      <c r="D6" s="107">
         <v>71.2</v>
       </c>
-      <c r="G6" s="139" t="s">
+      <c r="G6" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="140">
+      <c r="H6" s="106">
         <v>3.2</v>
       </c>
-      <c r="I6" s="141">
+      <c r="I6" s="107">
         <v>70.400000000000006</v>
       </c>
     </row>
@@ -24872,49 +24908,49 @@
       <c r="N8" s="98"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="142" t="s">
+      <c r="A9" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="143"/>
-      <c r="C9" s="144">
+      <c r="B9" s="109"/>
+      <c r="C9" s="110">
         <v>0.967391</v>
       </c>
       <c r="D9" s="89"/>
-      <c r="G9" s="145"/>
-      <c r="H9" s="146">
+      <c r="G9" s="111"/>
+      <c r="H9" s="112">
         <v>0.95652199999999998</v>
       </c>
-      <c r="I9" s="147"/>
+      <c r="I9" s="113"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1">
-      <c r="A10" s="148" t="s">
+      <c r="A10" s="114" t="s">
         <v>87</v>
       </c>
       <c r="B10" s="24"/>
-      <c r="C10" s="149">
+      <c r="C10" s="115">
         <v>3.1202000000000001E-2</v>
       </c>
       <c r="D10" s="91"/>
       <c r="G10" s="24"/>
-      <c r="H10" s="150">
+      <c r="H10" s="116">
         <v>3.1962999999999998E-2</v>
       </c>
-      <c r="I10" s="151"/>
+      <c r="I10" s="117"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1">
-      <c r="I12" s="152"/>
+      <c r="I12" s="118"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1">
-      <c r="A13" s="153" t="s">
+      <c r="A13" s="119" t="s">
         <v>88</v>
       </c>
       <c r="B13" s="39"/>
-      <c r="C13" s="154">
+      <c r="C13" s="120">
         <v>3.1706999999999999E-2</v>
       </c>
       <c r="D13" s="43"/>
       <c r="G13" s="39"/>
-      <c r="H13" s="154">
+      <c r="H13" s="120">
         <v>3.6097999999999998E-2</v>
       </c>
       <c r="I13" s="43"/>
@@ -24924,7 +24960,7 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="152"/>
+      <c r="A14" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -28501,10 +28537,10 @@
   <sheetData>
     <row r="1" spans="2:6" s="70" customFormat="1"/>
     <row r="2" spans="2:6">
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="154" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="121"/>
+      <c r="C2" s="154"/>
       <c r="D2" s="30"/>
     </row>
     <row r="3" spans="2:6">
@@ -28597,6 +28633,176 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0DF354-B4C5-4987-AD53-701F83618ECD}">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="8" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15" thickBot="1">
+      <c r="B1" s="145" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="146"/>
+      <c r="D1" s="147"/>
+      <c r="G1" s="145" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="146"/>
+      <c r="I1" s="147"/>
+    </row>
+    <row r="2" spans="1:16" ht="15" thickBot="1"/>
+    <row r="3" spans="1:16" ht="15" thickBot="1">
+      <c r="A3" s="74"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="148" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="149"/>
+      <c r="E3" s="99"/>
+      <c r="H3" s="150" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="151"/>
+    </row>
+    <row r="4" spans="1:16" ht="15" thickBot="1">
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="100" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="101" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="74"/>
+      <c r="H4" s="100" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="101" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="152" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" s="102" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="157">
+        <v>0.61658500000000005</v>
+      </c>
+      <c r="D5" s="158">
+        <v>2.4389999999999998E-2</v>
+      </c>
+      <c r="G5" s="102" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="157">
+        <v>0.61902400000000002</v>
+      </c>
+      <c r="I5" s="158">
+        <v>2.1950999999999998E-2</v>
+      </c>
+      <c r="O5" s="121"/>
+      <c r="P5" s="121"/>
+    </row>
+    <row r="6" spans="1:16" ht="15" thickBot="1">
+      <c r="A6" s="153"/>
+      <c r="B6" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="159">
+        <v>7.8050000000000003E-3</v>
+      </c>
+      <c r="D6" s="160">
+        <v>0.35121999999999998</v>
+      </c>
+      <c r="G6" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="159">
+        <v>1.1220000000000001E-2</v>
+      </c>
+      <c r="I6" s="160">
+        <v>0.34780499999999998</v>
+      </c>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="O7" s="121"/>
+      <c r="P7" s="121"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" thickBot="1"/>
+    <row r="9" spans="1:16">
+      <c r="A9" s="108" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="109"/>
+      <c r="C9" s="163">
+        <v>0.97826100000000005</v>
+      </c>
+      <c r="D9" s="89"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="161">
+        <v>0.96875</v>
+      </c>
+      <c r="I9" s="113"/>
+    </row>
+    <row r="10" spans="1:16" ht="15" thickBot="1">
+      <c r="A10" s="114" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="164">
+        <v>3.8052000000000002E-2</v>
+      </c>
+      <c r="D10" s="91"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="162">
+        <v>3.4247E-2</v>
+      </c>
+      <c r="I10" s="117"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" thickBot="1">
+      <c r="I12" s="118"/>
+    </row>
+    <row r="13" spans="1:16" ht="15" thickBot="1">
+      <c r="A13" s="119" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="122">
+        <v>3.2195000000000001E-2</v>
+      </c>
+      <c r="D13" s="43"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="122">
+        <v>3.3170999999999999E-2</v>
+      </c>
+      <c r="I13" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="H3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91D1BD3-6FA7-4787-B696-04D3642D0AA5}">
   <dimension ref="A1:U30"/>
   <sheetViews>
@@ -29035,7 +29241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE3B66D-7BD8-4F2A-9287-C113CF501316}">
   <dimension ref="A1:U30"/>
   <sheetViews>
@@ -29294,10 +29500,10 @@
       <c r="D15" s="4">
         <v>4.390244</v>
       </c>
-      <c r="M15" s="122" t="s">
+      <c r="M15" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="N15" s="123"/>
+      <c r="N15" s="156"/>
     </row>
     <row r="16" spans="1:21" ht="15" thickBot="1">
       <c r="A16" s="1" t="s">
@@ -29358,10 +29564,10 @@
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="122" t="s">
+      <c r="M19" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="N19" s="123"/>
+      <c r="N19" s="156"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickBot="1">
       <c r="A20" s="2"/>
@@ -29536,7 +29742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6AA21E-70DE-47C0-9B79-6D95FAF31B83}">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
@@ -29773,10 +29979,10 @@
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="122" t="s">
+      <c r="M13" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="N13" s="123"/>
+      <c r="N13" s="156"/>
     </row>
     <row r="14" spans="1:21" ht="15" thickBot="1">
       <c r="A14" s="2"/>
@@ -31051,17 +31257,17 @@
         <v>4.88</v>
       </c>
       <c r="L10" s="24"/>
-      <c r="M10" s="102" t="s">
+      <c r="M10" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="103"/>
-      <c r="O10" s="103"/>
-      <c r="P10" s="103"/>
-      <c r="Q10" s="103"/>
-      <c r="R10" s="103"/>
-      <c r="S10" s="103"/>
-      <c r="T10" s="103"/>
-      <c r="U10" s="104"/>
+      <c r="N10" s="127"/>
+      <c r="O10" s="127"/>
+      <c r="P10" s="127"/>
+      <c r="Q10" s="127"/>
+      <c r="R10" s="127"/>
+      <c r="S10" s="127"/>
+      <c r="T10" s="127"/>
+      <c r="U10" s="128"/>
       <c r="W10" s="31"/>
       <c r="X10" s="30"/>
       <c r="Y10" s="30"/>
@@ -31138,23 +31344,23 @@
         <v>8</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="M12" s="99" t="s">
+      <c r="M12" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="N12" s="100"/>
-      <c r="O12" s="100"/>
-      <c r="P12" s="100"/>
-      <c r="Q12" s="101"/>
-      <c r="W12" s="105" t="s">
+      <c r="N12" s="124"/>
+      <c r="O12" s="124"/>
+      <c r="P12" s="124"/>
+      <c r="Q12" s="125"/>
+      <c r="W12" s="129" t="s">
         <v>21</v>
       </c>
-      <c r="X12" s="106"/>
-      <c r="Y12" s="106"/>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
-      <c r="AB12" s="106"/>
-      <c r="AC12" s="106"/>
-      <c r="AD12" s="107"/>
+      <c r="X12" s="130"/>
+      <c r="Y12" s="130"/>
+      <c r="Z12" s="130"/>
+      <c r="AA12" s="130"/>
+      <c r="AB12" s="130"/>
+      <c r="AC12" s="130"/>
+      <c r="AD12" s="131"/>
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="3">
@@ -37967,16 +38173,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="108" t="s">
+      <c r="M1" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
+      <c r="N1" s="132"/>
+      <c r="O1" s="132"/>
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
+      <c r="R1" s="132"/>
+      <c r="S1" s="132"/>
+      <c r="T1" s="132"/>
       <c r="U1" s="10" t="s">
         <v>12</v>
       </c>
@@ -41873,16 +42079,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="108" t="s">
+      <c r="M1" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
+      <c r="N1" s="132"/>
+      <c r="O1" s="132"/>
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
+      <c r="R1" s="132"/>
+      <c r="S1" s="132"/>
+      <c r="T1" s="132"/>
       <c r="U1" s="10" t="s">
         <v>12</v>
       </c>
@@ -45767,16 +45973,16 @@
         <v>0</v>
       </c>
       <c r="L1" s="39"/>
-      <c r="M1" s="109" t="s">
+      <c r="M1" s="133" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="109"/>
-      <c r="O1" s="109"/>
-      <c r="P1" s="109"/>
-      <c r="Q1" s="109"/>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
-      <c r="T1" s="109"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
+      <c r="P1" s="133"/>
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="133"/>
+      <c r="T1" s="133"/>
       <c r="U1" s="28" t="s">
         <v>12</v>
       </c>
@@ -46727,17 +46933,17 @@
         <v>2</v>
       </c>
       <c r="L11" s="24"/>
-      <c r="M11" s="102" t="s">
+      <c r="M11" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="N11" s="103"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="103"/>
-      <c r="Q11" s="103"/>
-      <c r="R11" s="103"/>
-      <c r="S11" s="103"/>
-      <c r="T11" s="103"/>
-      <c r="U11" s="104"/>
+      <c r="N11" s="127"/>
+      <c r="O11" s="127"/>
+      <c r="P11" s="127"/>
+      <c r="Q11" s="127"/>
+      <c r="R11" s="127"/>
+      <c r="S11" s="127"/>
+      <c r="T11" s="127"/>
+      <c r="U11" s="128"/>
       <c r="W11" s="31"/>
       <c r="X11" s="30"/>
       <c r="Y11" s="30"/>
@@ -46846,16 +47052,16 @@
       <c r="K13" s="4">
         <v>6.8292679999999999</v>
       </c>
-      <c r="W13" s="110" t="s">
+      <c r="W13" s="134" t="s">
         <v>21</v>
       </c>
-      <c r="X13" s="111"/>
-      <c r="Y13" s="111"/>
-      <c r="Z13" s="111"/>
-      <c r="AA13" s="111"/>
-      <c r="AB13" s="111"/>
-      <c r="AC13" s="111"/>
-      <c r="AD13" s="112"/>
+      <c r="X13" s="135"/>
+      <c r="Y13" s="135"/>
+      <c r="Z13" s="135"/>
+      <c r="AA13" s="135"/>
+      <c r="AB13" s="135"/>
+      <c r="AC13" s="135"/>
+      <c r="AD13" s="136"/>
     </row>
     <row r="14" spans="1:30" ht="15" thickBot="1">
       <c r="A14" s="3">
@@ -46891,13 +47097,13 @@
       <c r="K14" s="4">
         <v>6.3414630000000001</v>
       </c>
-      <c r="M14" s="99" t="s">
+      <c r="M14" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="N14" s="100"/>
-      <c r="O14" s="100"/>
-      <c r="P14" s="100"/>
-      <c r="Q14" s="101"/>
+      <c r="N14" s="124"/>
+      <c r="O14" s="124"/>
+      <c r="P14" s="124"/>
+      <c r="Q14" s="125"/>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="3">

</xml_diff>

<commit_message>
absolute angle opt rank
</commit_message>
<xml_diff>
--- a/CancerSVM_dbscan.xlsx
+++ b/CancerSVM_dbscan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shukl\Documents\GitHub\CancerAceFiltering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C22603-D0E1-429F-A4BE-B943D62B3D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2C24B3-4742-4A08-9858-8728E89852B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="16" activeTab="20" xr2:uid="{17001702-3C6F-4149-BC22-539ABEDFA4DC}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="106">
   <si>
     <t>---------split 1 --------------------</t>
   </si>
@@ -548,6 +548,18 @@
   <si>
     <t>diff</t>
   </si>
+  <si>
+    <t>L1 knee error</t>
+  </si>
+  <si>
+    <t>L1 20% excision</t>
+  </si>
+  <si>
+    <t>knee opt rank error</t>
+  </si>
+  <si>
+    <t>knee opt rank angle</t>
+  </si>
 </sst>
 </file>
 
@@ -662,7 +674,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -768,6 +780,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1198,7 +1216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1500,7 +1518,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1543,6 +1560,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1559,12 +1582,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1597,40 +1614,16 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1639,10 +1632,19 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1654,13 +1656,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1669,7 +1668,62 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -11311,16 +11365,16 @@
         <v>0</v>
       </c>
       <c r="L1" s="39"/>
-      <c r="M1" s="150" t="s">
+      <c r="M1" s="149" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="150"/>
-      <c r="O1" s="150"/>
-      <c r="P1" s="150"/>
-      <c r="Q1" s="150"/>
-      <c r="R1" s="150"/>
-      <c r="S1" s="150"/>
-      <c r="T1" s="150"/>
+      <c r="N1" s="149"/>
+      <c r="O1" s="149"/>
+      <c r="P1" s="149"/>
+      <c r="Q1" s="149"/>
+      <c r="R1" s="149"/>
+      <c r="S1" s="149"/>
+      <c r="T1" s="149"/>
       <c r="U1" s="28" t="s">
         <v>12</v>
       </c>
@@ -12271,17 +12325,17 @@
         <v>2</v>
       </c>
       <c r="L11" s="24"/>
-      <c r="M11" s="143" t="s">
+      <c r="M11" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="144"/>
-      <c r="O11" s="144"/>
-      <c r="P11" s="144"/>
-      <c r="Q11" s="144"/>
-      <c r="R11" s="144"/>
-      <c r="S11" s="144"/>
-      <c r="T11" s="144"/>
-      <c r="U11" s="145"/>
+      <c r="N11" s="143"/>
+      <c r="O11" s="143"/>
+      <c r="P11" s="143"/>
+      <c r="Q11" s="143"/>
+      <c r="R11" s="143"/>
+      <c r="S11" s="143"/>
+      <c r="T11" s="143"/>
+      <c r="U11" s="144"/>
       <c r="W11" s="31"/>
       <c r="X11" s="30"/>
       <c r="Y11" s="30"/>
@@ -12390,16 +12444,16 @@
       <c r="K13" s="4">
         <v>6.8292679999999999</v>
       </c>
-      <c r="W13" s="151" t="s">
+      <c r="W13" s="150" t="s">
         <v>21</v>
       </c>
-      <c r="X13" s="152"/>
-      <c r="Y13" s="152"/>
-      <c r="Z13" s="152"/>
-      <c r="AA13" s="152"/>
-      <c r="AB13" s="152"/>
-      <c r="AC13" s="152"/>
-      <c r="AD13" s="153"/>
+      <c r="X13" s="151"/>
+      <c r="Y13" s="151"/>
+      <c r="Z13" s="151"/>
+      <c r="AA13" s="151"/>
+      <c r="AB13" s="151"/>
+      <c r="AC13" s="151"/>
+      <c r="AD13" s="152"/>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="3">
@@ -16096,16 +16150,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="149" t="s">
+      <c r="M1" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
-      <c r="P1" s="149"/>
-      <c r="Q1" s="149"/>
-      <c r="R1" s="149"/>
-      <c r="S1" s="149"/>
-      <c r="T1" s="149"/>
+      <c r="N1" s="148"/>
+      <c r="O1" s="148"/>
+      <c r="P1" s="148"/>
+      <c r="Q1" s="148"/>
+      <c r="R1" s="148"/>
+      <c r="S1" s="148"/>
+      <c r="T1" s="148"/>
       <c r="U1" s="10" t="s">
         <v>12</v>
       </c>
@@ -20002,16 +20056,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="149" t="s">
+      <c r="M1" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
-      <c r="P1" s="149"/>
-      <c r="Q1" s="149"/>
-      <c r="R1" s="149"/>
-      <c r="S1" s="149"/>
-      <c r="T1" s="149"/>
+      <c r="N1" s="148"/>
+      <c r="O1" s="148"/>
+      <c r="P1" s="148"/>
+      <c r="Q1" s="148"/>
+      <c r="R1" s="148"/>
+      <c r="S1" s="148"/>
+      <c r="T1" s="148"/>
       <c r="U1" s="10" t="s">
         <v>12</v>
       </c>
@@ -24806,26 +24860,26 @@
     <row r="2" spans="2:12" ht="15" thickBot="1">
       <c r="B2" s="73"/>
       <c r="C2" s="73"/>
-      <c r="D2" s="160" t="s">
+      <c r="D2" s="153" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="161"/>
+      <c r="E2" s="154"/>
       <c r="F2" s="76"/>
-      <c r="J2" s="160" t="s">
+      <c r="J2" s="153" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="161"/>
+      <c r="K2" s="154"/>
     </row>
     <row r="3" spans="2:12" ht="14.55" customHeight="1">
-      <c r="D3" s="156" t="s">
+      <c r="D3" s="157" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="157"/>
+      <c r="E3" s="158"/>
       <c r="F3" s="86"/>
-      <c r="J3" s="156" t="s">
+      <c r="J3" s="157" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="157"/>
+      <c r="K3" s="158"/>
     </row>
     <row r="4" spans="2:12" ht="15" thickBot="1">
       <c r="D4" s="77" t="s">
@@ -24843,7 +24897,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="14.55" customHeight="1">
-      <c r="B5" s="158" t="b">
+      <c r="B5" s="159" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="81" t="s">
@@ -24855,10 +24909,10 @@
       <c r="E5" s="80">
         <v>4.8</v>
       </c>
-      <c r="F5" s="154" t="s">
+      <c r="F5" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="158" t="b">
+      <c r="H5" s="159" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="81" t="s">
@@ -24870,12 +24924,12 @@
       <c r="K5" s="80">
         <v>4.2</v>
       </c>
-      <c r="L5" s="154" t="s">
+      <c r="L5" s="155" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15" thickBot="1">
-      <c r="B6" s="159"/>
+      <c r="B6" s="160"/>
       <c r="C6" s="82" t="s">
         <v>52</v>
       </c>
@@ -24885,8 +24939,8 @@
       <c r="E6" s="80">
         <v>72.8</v>
       </c>
-      <c r="F6" s="155"/>
-      <c r="H6" s="159"/>
+      <c r="F6" s="156"/>
+      <c r="H6" s="160"/>
       <c r="I6" s="82" t="s">
         <v>52</v>
       </c>
@@ -24896,7 +24950,7 @@
       <c r="K6" s="80">
         <v>70.400000000000006</v>
       </c>
-      <c r="L6" s="155"/>
+      <c r="L6" s="156"/>
     </row>
     <row r="7" spans="2:12" ht="28.8">
       <c r="D7" s="94" t="s">
@@ -25116,14 +25170,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -25156,26 +25210,26 @@
     <row r="2" spans="2:12" ht="15" thickBot="1">
       <c r="B2" s="73"/>
       <c r="C2" s="73"/>
-      <c r="D2" s="160" t="s">
+      <c r="D2" s="153" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="161"/>
+      <c r="E2" s="154"/>
       <c r="F2" s="76"/>
-      <c r="J2" s="160" t="s">
+      <c r="J2" s="153" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="161"/>
+      <c r="K2" s="154"/>
     </row>
     <row r="3" spans="2:12" ht="14.55" customHeight="1">
-      <c r="D3" s="156" t="s">
+      <c r="D3" s="157" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="157"/>
+      <c r="E3" s="158"/>
       <c r="F3" s="86"/>
-      <c r="J3" s="156" t="s">
+      <c r="J3" s="157" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="157"/>
+      <c r="K3" s="158"/>
     </row>
     <row r="4" spans="2:12" ht="15" thickBot="1">
       <c r="D4" s="77" t="s">
@@ -25193,7 +25247,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="14.55" customHeight="1">
-      <c r="B5" s="158" t="b">
+      <c r="B5" s="159" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="81" t="s">
@@ -25207,10 +25261,10 @@
         <f>D13</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="F5" s="154" t="s">
+      <c r="F5" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="158" t="b">
+      <c r="H5" s="159" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="81" t="s">
@@ -25222,12 +25276,12 @@
       <c r="K5" s="80">
         <v>4.2</v>
       </c>
-      <c r="L5" s="154" t="s">
+      <c r="L5" s="155" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15" thickBot="1">
-      <c r="B6" s="159"/>
+      <c r="B6" s="160"/>
       <c r="C6" s="82" t="s">
         <v>52</v>
       </c>
@@ -25239,8 +25293,8 @@
         <f>D14</f>
         <v>72.3</v>
       </c>
-      <c r="F6" s="155"/>
-      <c r="H6" s="159"/>
+      <c r="F6" s="156"/>
+      <c r="H6" s="160"/>
       <c r="I6" s="82" t="s">
         <v>52</v>
       </c>
@@ -25250,7 +25304,7 @@
       <c r="K6" s="80">
         <v>70.400000000000006</v>
       </c>
-      <c r="L6" s="155"/>
+      <c r="L6" s="156"/>
     </row>
     <row r="7" spans="2:12" ht="28.8">
       <c r="D7" s="94" t="s">
@@ -25497,30 +25551,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1">
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="161" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="163"/>
-      <c r="D1" s="164"/>
-      <c r="G1" s="162" t="s">
+      <c r="C1" s="162"/>
+      <c r="D1" s="163"/>
+      <c r="G1" s="161" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="163"/>
-      <c r="I1" s="164"/>
+      <c r="H1" s="162"/>
+      <c r="I1" s="163"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1"/>
     <row r="3" spans="1:14" ht="15" thickBot="1">
       <c r="A3" s="74"/>
       <c r="B3" s="74"/>
-      <c r="C3" s="165" t="s">
+      <c r="C3" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="166"/>
+      <c r="D3" s="165"/>
       <c r="E3" s="99"/>
-      <c r="H3" s="167" t="s">
+      <c r="H3" s="166" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="168"/>
+      <c r="I3" s="167"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
       <c r="A4" s="74"/>
@@ -25540,7 +25594,7 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="169" t="b">
+      <c r="A5" s="168" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="102" t="s">
@@ -25563,7 +25617,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1">
-      <c r="A6" s="170"/>
+      <c r="A6" s="169"/>
       <c r="B6" s="105" t="s">
         <v>52</v>
       </c>
@@ -29216,10 +29270,10 @@
   <sheetData>
     <row r="1" spans="2:6" s="70" customFormat="1"/>
     <row r="2" spans="2:6">
-      <c r="B2" s="171" t="s">
+      <c r="B2" s="170" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="171"/>
+      <c r="C2" s="170"/>
       <c r="D2" s="30"/>
     </row>
     <row r="3" spans="2:6">
@@ -29313,10 +29367,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0DF354-B4C5-4987-AD53-701F83618ECD}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -29324,37 +29378,41 @@
     <col min="2" max="2" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1">
-      <c r="C1" s="146" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="148"/>
-      <c r="E1" s="146" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="148"/>
-      <c r="G1" s="146" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="148"/>
-      <c r="I1" s="146" t="s">
+    <row r="1" spans="1:18" ht="15" thickBot="1">
+      <c r="C1" s="145" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="147"/>
+      <c r="E1" s="145" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="147"/>
+      <c r="G1" s="145" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="147"/>
+      <c r="I1" s="145" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="147"/>
+      <c r="K1" s="145" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="148"/>
-      <c r="L1" s="146" t="s">
+      <c r="L1" s="147"/>
+      <c r="M1" s="189" t="s">
         <v>99</v>
       </c>
-      <c r="M1" s="148"/>
-      <c r="N1" s="146" t="s">
+      <c r="N1" s="190"/>
+      <c r="O1" s="189" t="s">
         <v>98</v>
       </c>
-      <c r="O1" s="148"/>
-      <c r="P1" s="146" t="s">
+      <c r="P1" s="190"/>
+      <c r="Q1" s="189" t="s">
         <v>100</v>
       </c>
-      <c r="Q1" s="148"/>
-    </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1">
+      <c r="R1" s="190"/>
+    </row>
+    <row r="2" spans="1:18" ht="15" thickBot="1">
       <c r="C2" s="121"/>
       <c r="D2" s="23"/>
       <c r="E2" s="121"/>
@@ -29363,46 +29421,52 @@
       <c r="H2" s="23"/>
       <c r="I2" s="121"/>
       <c r="J2" s="23"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="121"/>
-      <c r="Q2" s="23"/>
-    </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" thickBot="1">
+      <c r="K2" s="121"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="191"/>
+      <c r="N2" s="192"/>
+      <c r="O2" s="191"/>
+      <c r="P2" s="192"/>
+      <c r="Q2" s="191"/>
+      <c r="R2" s="192"/>
+    </row>
+    <row r="3" spans="1:18" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="74"/>
       <c r="B3" s="74"/>
-      <c r="C3" s="165" t="s">
+      <c r="C3" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="166"/>
-      <c r="E3" s="165" t="s">
+      <c r="D3" s="165"/>
+      <c r="E3" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="166"/>
-      <c r="G3" s="165" t="s">
+      <c r="F3" s="165"/>
+      <c r="G3" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="166"/>
-      <c r="I3" s="165" t="s">
+      <c r="H3" s="165"/>
+      <c r="I3" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="166"/>
-      <c r="L3" s="165" t="s">
+      <c r="J3" s="165"/>
+      <c r="K3" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="M3" s="166"/>
-      <c r="N3" s="165" t="s">
+      <c r="L3" s="165"/>
+      <c r="M3" s="193" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="166"/>
-      <c r="P3" s="167" t="s">
+      <c r="N3" s="194"/>
+      <c r="O3" s="193" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="173"/>
-    </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1">
+      <c r="P3" s="194"/>
+      <c r="Q3" s="193" t="s">
+        <v>53</v>
+      </c>
+      <c r="R3" s="194"/>
+    </row>
+    <row r="4" spans="1:18" ht="15" thickBot="1">
       <c r="A4" s="74"/>
       <c r="B4" s="74"/>
       <c r="C4" s="100" t="s">
@@ -29429,27 +29493,33 @@
       <c r="J4" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="100" t="s">
+      <c r="K4" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="M4" s="101" t="s">
+      <c r="L4" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="N4" s="100" t="s">
+      <c r="M4" s="195" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="101" t="s">
+      <c r="N4" s="196" t="s">
         <v>52</v>
       </c>
-      <c r="P4" s="100" t="s">
+      <c r="O4" s="195" t="s">
         <v>51</v>
       </c>
-      <c r="Q4" s="101" t="s">
+      <c r="P4" s="196" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1">
-      <c r="A5" s="169" t="b">
+      <c r="Q4" s="195" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="196" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15" thickBot="1">
+      <c r="A5" s="168" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="102" t="s">
@@ -29474,32 +29544,38 @@
         <v>4.2410000000000003E-2</v>
       </c>
       <c r="I5" s="133">
+        <v>0.95684499999999995</v>
+      </c>
+      <c r="J5" s="134">
+        <v>4.3154999999999999E-2</v>
+      </c>
+      <c r="K5" s="133">
         <v>0.96428599999999998</v>
       </c>
-      <c r="J5" s="134">
+      <c r="L5" s="134">
         <v>3.5714000000000003E-2</v>
       </c>
-      <c r="L5" s="133">
+      <c r="M5" s="197">
         <v>0.96428599999999998</v>
       </c>
-      <c r="M5" s="134">
+      <c r="N5" s="198">
         <v>3.5714000000000003E-2</v>
       </c>
-      <c r="N5" s="133">
+      <c r="O5" s="197">
         <v>0.95833299999999999</v>
       </c>
-      <c r="O5" s="134">
+      <c r="P5" s="198">
         <v>4.1667000000000003E-2</v>
       </c>
-      <c r="P5" s="133">
+      <c r="Q5" s="197">
         <v>0.95758900000000002</v>
       </c>
-      <c r="Q5" s="134">
+      <c r="R5" s="198">
         <v>4.2410999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1">
-      <c r="A6" s="170"/>
+    <row r="6" spans="1:18" ht="15" thickBot="1">
+      <c r="A6" s="169"/>
       <c r="B6" s="105" t="s">
         <v>52</v>
       </c>
@@ -29522,31 +29598,37 @@
         <v>0.99008499999999999</v>
       </c>
       <c r="I6" s="135">
+        <v>1.2748000000000001E-2</v>
+      </c>
+      <c r="J6" s="136">
+        <v>0.98725200000000002</v>
+      </c>
+      <c r="K6" s="135">
         <v>2.2662999999999999E-2</v>
       </c>
-      <c r="J6" s="136">
+      <c r="L6" s="136">
         <v>0.97733700000000001</v>
       </c>
-      <c r="L6" s="135">
+      <c r="M6" s="199">
         <v>2.2662999999999999E-2</v>
       </c>
-      <c r="M6" s="136">
+      <c r="N6" s="200">
         <v>0.97733700000000001</v>
       </c>
-      <c r="N6" s="135">
+      <c r="O6" s="199">
         <v>1.6997000000000002E-2</v>
       </c>
-      <c r="O6" s="136">
+      <c r="P6" s="200">
         <v>0.98300299999999996</v>
       </c>
-      <c r="P6" s="133">
+      <c r="Q6" s="197">
         <v>9.9150000000000002E-3</v>
       </c>
-      <c r="Q6" s="134">
+      <c r="R6" s="198">
         <v>0.99008499999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="C7" s="137"/>
       <c r="D7" s="138"/>
       <c r="E7" s="137"/>
@@ -29555,14 +29637,16 @@
       <c r="H7" s="138"/>
       <c r="I7" s="137"/>
       <c r="J7" s="138"/>
-      <c r="L7" s="137"/>
-      <c r="M7" s="138"/>
-      <c r="N7" s="137"/>
-      <c r="O7" s="138"/>
-      <c r="P7" s="137"/>
-      <c r="Q7" s="138"/>
-    </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1">
+      <c r="K7" s="137"/>
+      <c r="L7" s="138"/>
+      <c r="M7" s="201"/>
+      <c r="N7" s="202"/>
+      <c r="O7" s="201"/>
+      <c r="P7" s="202"/>
+      <c r="Q7" s="201"/>
+      <c r="R7" s="202"/>
+    </row>
+    <row r="8" spans="1:18" ht="15" thickBot="1">
       <c r="C8" s="137"/>
       <c r="D8" s="138"/>
       <c r="E8" s="137"/>
@@ -29571,228 +29655,209 @@
       <c r="H8" s="138"/>
       <c r="I8" s="137"/>
       <c r="J8" s="138"/>
-      <c r="L8" s="137"/>
-      <c r="M8" s="138"/>
-      <c r="N8" s="137"/>
-      <c r="O8" s="138"/>
-      <c r="P8" s="137"/>
-      <c r="Q8" s="138"/>
-    </row>
-    <row r="9" spans="1:17" ht="15" thickBot="1">
+      <c r="K8" s="137"/>
+      <c r="L8" s="138"/>
+      <c r="M8" s="201"/>
+      <c r="N8" s="202"/>
+      <c r="O8" s="201"/>
+      <c r="P8" s="202"/>
+      <c r="Q8" s="201"/>
+      <c r="R8" s="202"/>
+    </row>
+    <row r="9" spans="1:18" ht="15" thickBot="1">
       <c r="A9" s="122" t="s">
         <v>86</v>
       </c>
       <c r="B9" s="109"/>
-      <c r="C9" s="180">
+      <c r="C9" s="171">
         <v>0.99291799999999997</v>
       </c>
-      <c r="D9" s="175"/>
-      <c r="E9" s="180">
+      <c r="D9" s="172"/>
+      <c r="E9" s="171">
         <v>0.99716700000000003</v>
       </c>
-      <c r="F9" s="175"/>
-      <c r="G9" s="180">
+      <c r="F9" s="172"/>
+      <c r="G9" s="171">
         <v>0.99008499999999999</v>
       </c>
-      <c r="H9" s="175"/>
-      <c r="I9" s="180">
+      <c r="H9" s="172"/>
+      <c r="I9" s="171">
+        <v>0.98725200000000002</v>
+      </c>
+      <c r="J9" s="172"/>
+      <c r="K9" s="171">
         <v>0.97733700000000001</v>
       </c>
-      <c r="J9" s="175"/>
-      <c r="L9" s="182">
+      <c r="L9" s="172"/>
+      <c r="M9" s="203">
         <v>0.97733700000000001</v>
       </c>
-      <c r="M9" s="183"/>
-      <c r="N9" s="180">
+      <c r="N9" s="204"/>
+      <c r="O9" s="205">
         <v>0.98300299999999996</v>
       </c>
-      <c r="O9" s="174"/>
-      <c r="P9" s="174">
+      <c r="P9" s="206"/>
+      <c r="Q9" s="206">
         <v>0.99008499999999999</v>
       </c>
-      <c r="Q9" s="175"/>
-    </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1">
+      <c r="R9" s="207"/>
+    </row>
+    <row r="10" spans="1:18" ht="15" thickBot="1">
       <c r="A10" s="123" t="s">
         <v>87</v>
       </c>
       <c r="B10" s="124"/>
-      <c r="C10" s="196">
+      <c r="C10" s="173">
         <v>4.2410999999999997E-2</v>
       </c>
-      <c r="D10" s="177"/>
-      <c r="E10" s="196">
+      <c r="D10" s="174"/>
+      <c r="E10" s="173">
         <v>4.3899000000000001E-2</v>
       </c>
-      <c r="F10" s="177"/>
-      <c r="G10" s="196">
+      <c r="F10" s="174"/>
+      <c r="G10" s="173">
         <v>4.2410000000000003E-2</v>
       </c>
-      <c r="H10" s="177"/>
-      <c r="I10" s="196">
+      <c r="H10" s="174"/>
+      <c r="I10" s="173">
+        <v>4.3154999999999999E-2</v>
+      </c>
+      <c r="J10" s="174"/>
+      <c r="K10" s="173">
         <v>3.5714000000000003E-2</v>
       </c>
-      <c r="J10" s="177"/>
-      <c r="L10" s="181">
+      <c r="L10" s="174"/>
+      <c r="M10" s="208">
         <v>3.5714000000000003E-2</v>
       </c>
-      <c r="M10" s="176"/>
-      <c r="N10" s="181">
+      <c r="N10" s="209"/>
+      <c r="O10" s="208">
         <v>4.1667000000000003E-2</v>
       </c>
-      <c r="O10" s="176"/>
-      <c r="P10" s="176">
+      <c r="P10" s="209"/>
+      <c r="Q10" s="209">
         <v>4.2410999999999997E-2</v>
       </c>
-      <c r="Q10" s="177"/>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="C11" s="137"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="138"/>
-      <c r="G11" s="137"/>
-      <c r="H11" s="138"/>
-      <c r="I11" s="137"/>
-      <c r="J11" s="138"/>
-      <c r="L11" s="137"/>
-      <c r="M11" s="138"/>
-      <c r="N11" s="137"/>
-      <c r="O11" s="138"/>
-      <c r="P11" s="137"/>
-      <c r="Q11" s="138"/>
-    </row>
-    <row r="12" spans="1:17" ht="15" thickBot="1">
-      <c r="C12" s="137"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="137"/>
-      <c r="F12" s="139"/>
-      <c r="G12" s="137"/>
-      <c r="H12" s="139"/>
-      <c r="I12" s="137"/>
-      <c r="J12" s="139"/>
-      <c r="L12" s="137"/>
-      <c r="M12" s="138"/>
-      <c r="N12" s="137"/>
-      <c r="O12" s="138"/>
-      <c r="P12" s="137"/>
-      <c r="Q12" s="139"/>
-    </row>
-    <row r="13" spans="1:17" ht="15" thickBot="1">
-      <c r="A13" s="119"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="178"/>
-      <c r="D13" s="179"/>
-      <c r="E13" s="178"/>
-      <c r="F13" s="179"/>
-      <c r="G13" s="178"/>
-      <c r="H13" s="179"/>
-      <c r="I13" s="178"/>
-      <c r="J13" s="179"/>
-      <c r="L13" s="178"/>
-      <c r="M13" s="179"/>
-      <c r="N13" s="178"/>
-      <c r="O13" s="179"/>
-      <c r="P13" s="178"/>
-      <c r="Q13" s="179"/>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="L16" s="172" t="s">
+      <c r="R10" s="210"/>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="M13" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="M16" s="172"/>
-      <c r="N16" s="172"/>
-      <c r="O16" s="172"/>
-      <c r="P16" s="172"/>
-      <c r="Q16" s="172"/>
-    </row>
-    <row r="17" spans="4:10" ht="15" thickBot="1"/>
-    <row r="18" spans="4:10" ht="15" thickBot="1">
-      <c r="I18" s="146"/>
-      <c r="J18" s="148"/>
-    </row>
-    <row r="19" spans="4:10" ht="15" thickBot="1">
-      <c r="I19" s="121"/>
-      <c r="J19" s="23"/>
-    </row>
-    <row r="20" spans="4:10" ht="15" thickBot="1">
-      <c r="I20" s="165"/>
-      <c r="J20" s="166"/>
-    </row>
-    <row r="21" spans="4:10" ht="15" thickBot="1">
-      <c r="D21" s="184"/>
-      <c r="E21" s="185"/>
-      <c r="I21" s="100"/>
-      <c r="J21" s="101"/>
-    </row>
-    <row r="22" spans="4:10">
-      <c r="I22" s="133"/>
-      <c r="J22" s="134"/>
-    </row>
-    <row r="23" spans="4:10" ht="15" thickBot="1">
-      <c r="I23" s="135"/>
-      <c r="J23" s="136"/>
-    </row>
-    <row r="24" spans="4:10">
-      <c r="I24" s="137"/>
-      <c r="J24" s="138"/>
-    </row>
-    <row r="25" spans="4:10" ht="15" thickBot="1">
-      <c r="I25" s="137"/>
-      <c r="J25" s="138"/>
-    </row>
-    <row r="26" spans="4:10">
-      <c r="I26" s="180"/>
-      <c r="J26" s="175"/>
-    </row>
-    <row r="27" spans="4:10" ht="15" thickBot="1">
-      <c r="I27" s="196"/>
-      <c r="J27" s="177"/>
+      <c r="N13" s="177"/>
+      <c r="O13" s="177"/>
+      <c r="P13" s="177"/>
+      <c r="Q13" s="177"/>
+      <c r="R13" s="177"/>
+    </row>
+    <row r="14" spans="1:18" ht="15" thickBot="1"/>
+    <row r="15" spans="1:18" ht="15" thickBot="1">
+      <c r="I15" s="145"/>
+      <c r="J15" s="147"/>
+      <c r="K15" s="145"/>
+      <c r="L15" s="147"/>
+    </row>
+    <row r="16" spans="1:18" ht="15" thickBot="1">
+      <c r="I16" s="121"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="121"/>
+      <c r="L16" s="23"/>
+    </row>
+    <row r="17" spans="4:12" ht="15" thickBot="1">
+      <c r="I17" s="164"/>
+      <c r="J17" s="165"/>
+      <c r="K17" s="164"/>
+      <c r="L17" s="165"/>
+    </row>
+    <row r="18" spans="4:12" ht="15" thickBot="1">
+      <c r="D18" s="175"/>
+      <c r="E18" s="176"/>
+      <c r="I18" s="100"/>
+      <c r="J18" s="101"/>
+      <c r="K18" s="100"/>
+      <c r="L18" s="101"/>
+    </row>
+    <row r="19" spans="4:12">
+      <c r="I19" s="133"/>
+      <c r="J19" s="134"/>
+      <c r="K19" s="133"/>
+      <c r="L19" s="134"/>
+    </row>
+    <row r="20" spans="4:12" ht="15" thickBot="1">
+      <c r="I20" s="135"/>
+      <c r="J20" s="136"/>
+      <c r="K20" s="135"/>
+      <c r="L20" s="136"/>
+    </row>
+    <row r="21" spans="4:12">
+      <c r="I21" s="137"/>
+      <c r="J21" s="138"/>
+      <c r="K21" s="137"/>
+      <c r="L21" s="138"/>
+    </row>
+    <row r="22" spans="4:12" ht="15" thickBot="1">
+      <c r="I22" s="137"/>
+      <c r="J22" s="138"/>
+      <c r="K22" s="137"/>
+      <c r="L22" s="138"/>
+    </row>
+    <row r="23" spans="4:12">
+      <c r="I23" s="171"/>
+      <c r="J23" s="172"/>
+      <c r="K23" s="171"/>
+      <c r="L23" s="172"/>
+    </row>
+    <row r="24" spans="4:12" ht="15" thickBot="1">
+      <c r="I24" s="173"/>
+      <c r="J24" s="174"/>
+      <c r="K24" s="173"/>
+      <c r="L24" s="174"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
+  <mergeCells count="43">
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="M13:R13"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="L16:Q16"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -29810,22 +29875,22 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1">
-      <c r="C1" s="146" t="s">
+      <c r="C1" s="145" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="148"/>
-      <c r="E1" s="146" t="s">
+      <c r="D1" s="147"/>
+      <c r="E1" s="145" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="148"/>
-      <c r="G1" s="146" t="s">
+      <c r="F1" s="147"/>
+      <c r="G1" s="145" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="148"/>
-      <c r="I1" s="146" t="s">
+      <c r="H1" s="147"/>
+      <c r="I1" s="145" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="148"/>
+      <c r="J1" s="147"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" thickBot="1">
       <c r="C2" s="121"/>
@@ -29840,22 +29905,22 @@
     <row r="3" spans="1:10" ht="15" thickBot="1">
       <c r="A3" s="74"/>
       <c r="B3" s="74"/>
-      <c r="C3" s="167" t="s">
+      <c r="C3" s="166" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="173"/>
-      <c r="E3" s="165" t="s">
+      <c r="D3" s="178"/>
+      <c r="E3" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="166"/>
-      <c r="G3" s="167" t="s">
+      <c r="F3" s="165"/>
+      <c r="G3" s="166" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="173"/>
-      <c r="I3" s="167" t="s">
+      <c r="H3" s="178"/>
+      <c r="I3" s="166" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="173"/>
+      <c r="J3" s="178"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1">
       <c r="A4" s="74"/>
@@ -29886,7 +29951,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1">
-      <c r="A5" s="169" t="b">
+      <c r="A5" s="168" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="102" t="s">
@@ -29918,7 +29983,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1">
-      <c r="A6" s="170"/>
+      <c r="A6" s="169"/>
       <c r="B6" s="105" t="s">
         <v>52</v>
       </c>
@@ -29972,44 +30037,44 @@
         <v>86</v>
       </c>
       <c r="B9" s="109"/>
-      <c r="C9" s="192">
+      <c r="C9" s="180">
         <v>0.99433400000000005</v>
       </c>
-      <c r="D9" s="192"/>
-      <c r="E9" s="191">
+      <c r="D9" s="180"/>
+      <c r="E9" s="179">
         <v>0.97592100000000004</v>
       </c>
-      <c r="F9" s="192"/>
-      <c r="G9" s="192">
+      <c r="F9" s="180"/>
+      <c r="G9" s="180">
         <v>0.98016999999999999</v>
       </c>
-      <c r="H9" s="193"/>
-      <c r="I9" s="192">
+      <c r="H9" s="181"/>
+      <c r="I9" s="180">
         <v>0.97167099999999995</v>
       </c>
-      <c r="J9" s="193"/>
+      <c r="J9" s="181"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1">
       <c r="A10" s="123" t="s">
         <v>87</v>
       </c>
       <c r="B10" s="124"/>
-      <c r="C10" s="189">
+      <c r="C10" s="183">
         <v>6.9195999999999994E-2</v>
       </c>
-      <c r="D10" s="189"/>
-      <c r="E10" s="188">
+      <c r="D10" s="183"/>
+      <c r="E10" s="182">
         <v>3.5714000000000003E-2</v>
       </c>
-      <c r="F10" s="189"/>
-      <c r="G10" s="189">
+      <c r="F10" s="183"/>
+      <c r="G10" s="183">
         <v>3.4225999999999999E-2</v>
       </c>
-      <c r="H10" s="190"/>
-      <c r="I10" s="189">
+      <c r="H10" s="184"/>
+      <c r="I10" s="183">
         <v>3.125E-2</v>
       </c>
-      <c r="J10" s="190"/>
+      <c r="J10" s="184"/>
     </row>
     <row r="11" spans="1:10">
       <c r="C11" s="129"/>
@@ -30036,22 +30101,22 @@
         <v>88</v>
       </c>
       <c r="B13" s="39"/>
-      <c r="C13" s="186">
+      <c r="C13" s="185">
         <v>4.7316999999999998E-2</v>
       </c>
-      <c r="D13" s="187"/>
-      <c r="E13" s="186">
+      <c r="D13" s="186"/>
+      <c r="E13" s="185">
         <v>3.1706999999999999E-2</v>
       </c>
-      <c r="F13" s="187"/>
-      <c r="G13" s="186">
+      <c r="F13" s="186"/>
+      <c r="G13" s="185">
         <v>2.9267999999999999E-2</v>
       </c>
-      <c r="H13" s="187"/>
-      <c r="I13" s="186">
+      <c r="H13" s="186"/>
+      <c r="I13" s="185">
         <v>3.0244E-2</v>
       </c>
-      <c r="J13" s="187"/>
+      <c r="J13" s="186"/>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" s="132" t="s">
@@ -30060,6 +30125,16 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="I1:J1"/>
@@ -30071,16 +30146,6 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -30856,10 +30921,10 @@
       <c r="D15" s="4">
         <v>4.390244</v>
       </c>
-      <c r="M15" s="194" t="s">
+      <c r="M15" s="187" t="s">
         <v>43</v>
       </c>
-      <c r="N15" s="195"/>
+      <c r="N15" s="188"/>
     </row>
     <row r="16" spans="1:21" ht="15" thickBot="1">
       <c r="A16" s="1" t="s">
@@ -30920,10 +30985,10 @@
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="194" t="s">
+      <c r="M19" s="187" t="s">
         <v>43</v>
       </c>
-      <c r="N19" s="195"/>
+      <c r="N19" s="188"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickBot="1">
       <c r="A20" s="2"/>
@@ -31335,10 +31400,10 @@
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="194" t="s">
+      <c r="M13" s="187" t="s">
         <v>43</v>
       </c>
-      <c r="N13" s="195"/>
+      <c r="N13" s="188"/>
     </row>
     <row r="14" spans="1:21" ht="15" thickBot="1">
       <c r="A14" s="2"/>
@@ -32613,17 +32678,17 @@
         <v>4.88</v>
       </c>
       <c r="L10" s="24"/>
-      <c r="M10" s="143" t="s">
+      <c r="M10" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="144"/>
-      <c r="O10" s="144"/>
-      <c r="P10" s="144"/>
-      <c r="Q10" s="144"/>
-      <c r="R10" s="144"/>
-      <c r="S10" s="144"/>
-      <c r="T10" s="144"/>
-      <c r="U10" s="145"/>
+      <c r="N10" s="143"/>
+      <c r="O10" s="143"/>
+      <c r="P10" s="143"/>
+      <c r="Q10" s="143"/>
+      <c r="R10" s="143"/>
+      <c r="S10" s="143"/>
+      <c r="T10" s="143"/>
+      <c r="U10" s="144"/>
       <c r="W10" s="31"/>
       <c r="X10" s="30"/>
       <c r="Y10" s="30"/>
@@ -32700,23 +32765,23 @@
         <v>8</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="M12" s="140" t="s">
+      <c r="M12" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="N12" s="141"/>
-      <c r="O12" s="141"/>
-      <c r="P12" s="141"/>
-      <c r="Q12" s="142"/>
-      <c r="W12" s="146" t="s">
+      <c r="N12" s="140"/>
+      <c r="O12" s="140"/>
+      <c r="P12" s="140"/>
+      <c r="Q12" s="141"/>
+      <c r="W12" s="145" t="s">
         <v>21</v>
       </c>
-      <c r="X12" s="147"/>
-      <c r="Y12" s="147"/>
-      <c r="Z12" s="147"/>
-      <c r="AA12" s="147"/>
-      <c r="AB12" s="147"/>
-      <c r="AC12" s="147"/>
-      <c r="AD12" s="148"/>
+      <c r="X12" s="146"/>
+      <c r="Y12" s="146"/>
+      <c r="Z12" s="146"/>
+      <c r="AA12" s="146"/>
+      <c r="AB12" s="146"/>
+      <c r="AC12" s="146"/>
+      <c r="AD12" s="147"/>
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="3">
@@ -39529,16 +39594,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="149" t="s">
+      <c r="M1" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
-      <c r="P1" s="149"/>
-      <c r="Q1" s="149"/>
-      <c r="R1" s="149"/>
-      <c r="S1" s="149"/>
-      <c r="T1" s="149"/>
+      <c r="N1" s="148"/>
+      <c r="O1" s="148"/>
+      <c r="P1" s="148"/>
+      <c r="Q1" s="148"/>
+      <c r="R1" s="148"/>
+      <c r="S1" s="148"/>
+      <c r="T1" s="148"/>
       <c r="U1" s="10" t="s">
         <v>12</v>
       </c>
@@ -43435,16 +43500,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="149" t="s">
+      <c r="M1" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
-      <c r="P1" s="149"/>
-      <c r="Q1" s="149"/>
-      <c r="R1" s="149"/>
-      <c r="S1" s="149"/>
-      <c r="T1" s="149"/>
+      <c r="N1" s="148"/>
+      <c r="O1" s="148"/>
+      <c r="P1" s="148"/>
+      <c r="Q1" s="148"/>
+      <c r="R1" s="148"/>
+      <c r="S1" s="148"/>
+      <c r="T1" s="148"/>
       <c r="U1" s="10" t="s">
         <v>12</v>
       </c>
@@ -47329,16 +47394,16 @@
         <v>0</v>
       </c>
       <c r="L1" s="39"/>
-      <c r="M1" s="150" t="s">
+      <c r="M1" s="149" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="150"/>
-      <c r="O1" s="150"/>
-      <c r="P1" s="150"/>
-      <c r="Q1" s="150"/>
-      <c r="R1" s="150"/>
-      <c r="S1" s="150"/>
-      <c r="T1" s="150"/>
+      <c r="N1" s="149"/>
+      <c r="O1" s="149"/>
+      <c r="P1" s="149"/>
+      <c r="Q1" s="149"/>
+      <c r="R1" s="149"/>
+      <c r="S1" s="149"/>
+      <c r="T1" s="149"/>
       <c r="U1" s="28" t="s">
         <v>12</v>
       </c>
@@ -48289,17 +48354,17 @@
         <v>2</v>
       </c>
       <c r="L11" s="24"/>
-      <c r="M11" s="143" t="s">
+      <c r="M11" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="N11" s="144"/>
-      <c r="O11" s="144"/>
-      <c r="P11" s="144"/>
-      <c r="Q11" s="144"/>
-      <c r="R11" s="144"/>
-      <c r="S11" s="144"/>
-      <c r="T11" s="144"/>
-      <c r="U11" s="145"/>
+      <c r="N11" s="143"/>
+      <c r="O11" s="143"/>
+      <c r="P11" s="143"/>
+      <c r="Q11" s="143"/>
+      <c r="R11" s="143"/>
+      <c r="S11" s="143"/>
+      <c r="T11" s="143"/>
+      <c r="U11" s="144"/>
       <c r="W11" s="31"/>
       <c r="X11" s="30"/>
       <c r="Y11" s="30"/>
@@ -48408,16 +48473,16 @@
       <c r="K13" s="4">
         <v>6.8292679999999999</v>
       </c>
-      <c r="W13" s="151" t="s">
+      <c r="W13" s="150" t="s">
         <v>21</v>
       </c>
-      <c r="X13" s="152"/>
-      <c r="Y13" s="152"/>
-      <c r="Z13" s="152"/>
-      <c r="AA13" s="152"/>
-      <c r="AB13" s="152"/>
-      <c r="AC13" s="152"/>
-      <c r="AD13" s="153"/>
+      <c r="X13" s="151"/>
+      <c r="Y13" s="151"/>
+      <c r="Z13" s="151"/>
+      <c r="AA13" s="151"/>
+      <c r="AB13" s="151"/>
+      <c r="AC13" s="151"/>
+      <c r="AD13" s="152"/>
     </row>
     <row r="14" spans="1:30" ht="15" thickBot="1">
       <c r="A14" s="3">
@@ -48453,13 +48518,13 @@
       <c r="K14" s="4">
         <v>6.3414630000000001</v>
       </c>
-      <c r="M14" s="140" t="s">
+      <c r="M14" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="N14" s="141"/>
-      <c r="O14" s="141"/>
-      <c r="P14" s="141"/>
-      <c r="Q14" s="142"/>
+      <c r="N14" s="140"/>
+      <c r="O14" s="140"/>
+      <c r="P14" s="140"/>
+      <c r="Q14" s="141"/>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="3">

</xml_diff>